<commit_message>
More data for $TOST
</commit_message>
<xml_diff>
--- a/Overview - Tech.xlsx
+++ b/Overview - Tech.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615BF1F2-2937-4DD9-A7E5-4EBAE5578AFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5C04DC-EECC-498F-84C6-AE324998C234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AFC643F4-9510-457F-8BC2-75D95EE8546E}"/>
   </bookViews>
@@ -23,18 +23,28 @@
     <externalReference r:id="rId6"/>
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
   <si>
     <t>Ticker</t>
   </si>
@@ -243,10 +253,13 @@
     <t>$TOST</t>
   </si>
   <si>
-    <t>Toast, Inc.</t>
-  </si>
-  <si>
     <t>Restaurant POS &amp; Management</t>
+  </si>
+  <si>
+    <t>Twillo Inc.</t>
+  </si>
+  <si>
+    <t>Toast Inc.</t>
   </si>
 </sst>
 </file>
@@ -434,7 +447,36 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -448,8 +490,11 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Financial Model"/>
@@ -587,8 +632,11 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Financial Model"/>
@@ -636,10 +684,10 @@
             <v>2595.5510000000004</v>
           </cell>
           <cell r="G11" t="str">
-            <v>Q224</v>
+            <v>Q324</v>
           </cell>
           <cell r="H11">
-            <v>45505</v>
+            <v>45596</v>
           </cell>
         </row>
         <row r="12">
@@ -707,15 +755,15 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -820,7 +868,121 @@
 </file>
 
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Financial Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="C6">
+            <v>31.25</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>562</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8">
+            <v>17562.5</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>1219</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>16343.5</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="C23" t="str">
+            <v>Boston, MA</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="C24">
+            <v>2011</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="C25">
+            <v>2021</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="C28">
+            <v>5500</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="C30" t="str">
+            <v>Q224</v>
+          </cell>
+          <cell r="D30">
+            <v>45511</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="C35">
+            <v>13.542478565861263</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="C36">
+            <v>4.0051311288483467</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="28">
+          <cell r="L28">
+            <v>0.23027375201288244</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="L29">
+            <v>4.0257648953301124E-3</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="L30">
+            <v>1.1272141706924315E-2</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="L31">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="L33">
+            <v>0.26993865030674846</v>
+          </cell>
+          <cell r="T33">
+            <v>0.6017595307917889</v>
+          </cell>
+          <cell r="U33">
+            <v>0.41523251556206509</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -923,8 +1085,8 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -933,6 +1095,11 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
+        <row r="6">
+          <cell r="C6">
+            <v>3.33</v>
+          </cell>
+        </row>
         <row r="7">
           <cell r="C7">
             <v>193.41571500000001</v>
@@ -1020,108 +1187,38 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Financial Model"/>
+      <sheetName val="Historical Projections"/>
+      <sheetName val="Price History"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="6">
-          <cell r="C6">
-            <v>31.25</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7">
-            <v>562</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="C8">
-            <v>17562.5</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>1219</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12">
-            <v>16343.5</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="C23" t="str">
-            <v>Boston, MA</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="C24">
-            <v>2011</v>
-          </cell>
-        </row>
         <row r="28">
-          <cell r="C28">
-            <v>5500</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="C30" t="str">
-            <v>Q224</v>
-          </cell>
-          <cell r="D30">
-            <v>45511</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="C35">
-            <v>13.542478565861263</v>
+          <cell r="C28" t="str">
+            <v>Q123</v>
+          </cell>
+          <cell r="D28">
+            <v>45055</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1">
-        <row r="28">
-          <cell r="L28">
-            <v>0.23027375201288244</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="L29">
-            <v>4.0257648953301124E-3</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="L30">
-            <v>1.1272141706924315E-2</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="L31">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="L33">
-            <v>0.26993865030674846</v>
-          </cell>
-          <cell r="S33">
-            <v>0.6017595307917889</v>
-          </cell>
-          <cell r="T33">
-            <v>0.41523251556206509</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1427,10 +1524,10 @@
   <dimension ref="B1:AL15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AB9" sqref="AB9"/>
+      <selection pane="bottomRight" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1442,7 +1539,7 @@
     <col min="6" max="6" width="9.140625" style="10"/>
     <col min="7" max="10" width="9.140625" style="8"/>
     <col min="11" max="11" width="9.140625" style="2"/>
-    <col min="12" max="12" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" style="15" bestFit="1" customWidth="1"/>
     <col min="13" max="15" width="0" style="19" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="9.140625" style="1"/>
     <col min="17" max="19" width="9.140625" style="12"/>
@@ -1464,6 +1561,7 @@
       <c r="F1" s="27" t="s">
         <v>60</v>
       </c>
+      <c r="L1" s="2"/>
     </row>
     <row r="2" spans="2:38" s="3" customFormat="1">
       <c r="B2" s="3" t="s">
@@ -1724,11 +1822,11 @@
       </c>
       <c r="K5" s="2" t="str">
         <f>+[2]Main!$G$11</f>
-        <v>Q224</v>
+        <v>Q324</v>
       </c>
       <c r="L5" s="15">
         <f>+[2]Main!$H$11</f>
-        <v>45505</v>
+        <v>45596</v>
       </c>
       <c r="M5" s="22">
         <f>+'[2]Financial Model'!$AX$26</f>
@@ -1912,14 +2010,13 @@
       <c r="F7" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="L7" s="15"/>
     </row>
     <row r="8" spans="2:38">
       <c r="B8" s="5" t="s">
         <v>68</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>37</v>
@@ -1928,88 +2025,104 @@
         <v>33</v>
       </c>
       <c r="F8" s="10">
-        <f>+[6]Main!$C$6</f>
+        <f>+[4]Main!$C$6</f>
         <v>31.25</v>
       </c>
       <c r="G8" s="8">
-        <f>+[6]Main!$C$7</f>
+        <f>+[4]Main!$C$7</f>
         <v>562</v>
       </c>
       <c r="H8" s="8">
-        <f>+[6]Main!$C$8</f>
+        <f>+[4]Main!$C$8</f>
         <v>17562.5</v>
       </c>
       <c r="I8" s="8">
-        <f>+[6]Main!$C$11</f>
+        <f>+[4]Main!$C$11</f>
         <v>1219</v>
       </c>
       <c r="J8" s="8">
-        <f>+[6]Main!$C$12</f>
+        <f>+[4]Main!$C$12</f>
         <v>16343.5</v>
       </c>
       <c r="K8" s="2" t="str">
-        <f>+[6]Main!$C$30</f>
+        <f>+[4]Main!$C$30</f>
         <v>Q224</v>
       </c>
       <c r="L8" s="15">
-        <f>+[6]Main!$D$30</f>
+        <f>+[4]Main!$D$30</f>
         <v>45511</v>
       </c>
       <c r="Q8" s="12">
-        <f>+[6]Main!$C$35</f>
+        <f>+[4]Main!$C$35</f>
         <v>13.542478565861263</v>
       </c>
+      <c r="R8" s="12">
+        <f>+[4]Main!$C$36</f>
+        <v>4.0051311288483467</v>
+      </c>
       <c r="U8" s="14">
-        <f>+'[6]Financial Model'!$L$28</f>
+        <f>+'[4]Financial Model'!$L$28</f>
         <v>0.23027375201288244</v>
       </c>
       <c r="V8" s="14">
-        <f>+'[6]Financial Model'!$L$29</f>
+        <f>+'[4]Financial Model'!$L$29</f>
         <v>4.0257648953301124E-3</v>
       </c>
       <c r="W8" s="14">
-        <f>+'[6]Financial Model'!$L$30</f>
+        <f>+'[4]Financial Model'!$L$30</f>
         <v>1.1272141706924315E-2</v>
       </c>
       <c r="X8" s="14">
-        <f>+'[6]Financial Model'!$L$31</f>
+        <f>+'[4]Financial Model'!$L$31</f>
         <v>0</v>
       </c>
       <c r="Z8" s="14">
-        <f>+'[6]Financial Model'!$L$33</f>
+        <f>+'[4]Financial Model'!$L$33</f>
         <v>0.26993865030674846</v>
       </c>
       <c r="AA8" s="14">
-        <f>+'[6]Financial Model'!$T$33</f>
+        <f>+'[4]Financial Model'!$U$33</f>
         <v>0.41523251556206509</v>
       </c>
       <c r="AB8" s="14">
-        <f>+'[6]Financial Model'!$S$33</f>
+        <f>+'[4]Financial Model'!$T$33</f>
         <v>0.6017595307917889</v>
       </c>
       <c r="AF8" s="20">
-        <f>+[6]Main!$C$28</f>
+        <f>+[4]Main!$C$28</f>
         <v>5500</v>
       </c>
       <c r="AG8" s="2">
-        <f>+[6]Main!$C$24</f>
+        <f>+[4]Main!$C$24</f>
         <v>2011</v>
       </c>
+      <c r="AH8" s="2">
+        <f>+[4]Main!$C$25</f>
+        <v>2021</v>
+      </c>
       <c r="AI8" s="2" t="str">
-        <f>+[6]Main!$C$23</f>
+        <f>+[4]Main!$C$23</f>
         <v>Boston, MA</v>
       </c>
       <c r="AL8" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="2:38">
-      <c r="L9" s="15"/>
+        <v>69</v>
+      </c>
     </row>
     <row r="10" spans="2:38">
       <c r="B10" s="5" t="s">
         <v>67</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K10" s="2" t="str">
+        <f>+[7]Main!$C$28</f>
+        <v>Q123</v>
+      </c>
+      <c r="L10" s="15">
+        <f>+[7]Main!$D$28</f>
+        <v>45055</v>
+      </c>
     </row>
     <row r="12" spans="2:38">
       <c r="B12" s="5" t="s">
@@ -2025,11 +2138,11 @@
         <v>51</v>
       </c>
       <c r="F12" s="10">
-        <f>+[4]Main!$C$6*Currencies!C3</f>
+        <f>+[5]Main!$C$6*Currencies!C3</f>
         <v>12.851799999999999</v>
       </c>
       <c r="G12" s="8">
-        <f>+[4]Main!$C$7</f>
+        <f>+[5]Main!$C$7</f>
         <v>1016</v>
       </c>
       <c r="H12" s="8">
@@ -2037,7 +2150,7 @@
         <v>13057.4288</v>
       </c>
       <c r="I12" s="8">
-        <f>[4]Main!$C$11*Currencies!C3</f>
+        <f>[5]Main!$C$11*Currencies!C3</f>
         <v>-1029.6000000000001</v>
       </c>
       <c r="J12" s="8">
@@ -2045,67 +2158,67 @@
         <v>14087.0288</v>
       </c>
       <c r="K12" s="2" t="str">
-        <f>+[4]Main!$C$27</f>
+        <f>+[5]Main!$C$27</f>
         <v>H124</v>
       </c>
       <c r="L12" s="15">
-        <f>+[4]Main!$D$27</f>
+        <f>+[5]Main!$D$27</f>
         <v>45428</v>
       </c>
       <c r="Q12" s="12">
-        <f>[4]Main!$C$34</f>
+        <f>[5]Main!$C$34</f>
         <v>9.2317794117647036</v>
       </c>
       <c r="R12" s="12">
-        <f>[4]Main!$C$33</f>
+        <f>[5]Main!$C$33</f>
         <v>4.4660631391729657</v>
       </c>
       <c r="S12" s="12">
-        <f>+[4]Main!$C$32</f>
+        <f>+[5]Main!$C$32</f>
         <v>26.149764972535884</v>
       </c>
       <c r="U12" s="14">
-        <f>+'[4]Financial Model'!$M$20</f>
+        <f>+'[5]Financial Model'!$M$20</f>
         <v>0.92881944444444442</v>
       </c>
       <c r="V12" s="14">
-        <f>+'[4]Financial Model'!$M$21</f>
+        <f>+'[5]Financial Model'!$M$21</f>
         <v>0.18663194444444445</v>
       </c>
       <c r="W12" s="14">
-        <f>+'[4]Financial Model'!$M$22</f>
+        <f>+'[5]Financial Model'!$M$22</f>
         <v>0.13541666666666666</v>
       </c>
       <c r="X12" s="14">
-        <f>+'[4]Financial Model'!$M$23</f>
+        <f>+'[5]Financial Model'!$M$23</f>
         <v>0.23152709359605911</v>
       </c>
       <c r="Z12" s="14">
-        <f>+'[4]Financial Model'!$M$25</f>
+        <f>+'[5]Financial Model'!$M$25</f>
         <v>5.9797608095676136E-2</v>
       </c>
       <c r="AA12" s="14">
-        <f>+'[4]Financial Model'!$W$25</f>
+        <f>+'[5]Financial Model'!$W$25</f>
         <v>0.1217257318952234</v>
       </c>
       <c r="AB12" s="14">
-        <f>+'[4]Financial Model'!$V$25</f>
+        <f>+'[5]Financial Model'!$V$25</f>
         <v>5.4712892741061836E-2</v>
       </c>
       <c r="AC12" s="14">
-        <f>+'[4]Financial Model'!$U$25</f>
+        <f>+'[5]Financial Model'!$U$25</f>
         <v>-2.9952706253284278E-2</v>
       </c>
       <c r="AF12" s="20">
-        <f>+[4]Main!$C$26</f>
+        <f>+[5]Main!$C$26</f>
         <v>11565</v>
       </c>
       <c r="AG12" s="2">
-        <f>+[4]Main!$C$24</f>
+        <f>+[5]Main!$C$24</f>
         <v>1981</v>
       </c>
       <c r="AH12" s="2">
-        <f>+[4]Main!$C$25</f>
+        <f>+[5]Main!$C$25</f>
         <v>1989</v>
       </c>
       <c r="AI12" s="2" t="s">
@@ -2132,90 +2245,90 @@
         <v>33</v>
       </c>
       <c r="F13" s="10">
-        <f>+[4]Main!$C$6*Currencies!C3</f>
-        <v>12.851799999999999</v>
+        <f>+[6]Main!$C$6*Currencies!C3</f>
+        <v>4.3290000000000006</v>
       </c>
       <c r="G13" s="8">
-        <f>+[5]Main!$C$7</f>
+        <f>+[6]Main!$C$7</f>
         <v>193.41571500000001</v>
       </c>
       <c r="H13" s="8">
         <f>G13*F13</f>
-        <v>2485.7400860369999</v>
+        <v>837.29663023500018</v>
       </c>
       <c r="I13" s="8">
-        <f>[5]Main!$C$11*Currencies!D3</f>
+        <f>[6]Main!$C$11*Currencies!D3</f>
         <v>20.227692307692305</v>
       </c>
       <c r="J13" s="8">
         <f>H13-I13</f>
-        <v>2465.5123937293074</v>
+        <v>817.06893792730784</v>
       </c>
       <c r="K13" s="2" t="str">
-        <f>[5]Main!$C$30</f>
+        <f>[6]Main!$C$30</f>
         <v>H124</v>
       </c>
       <c r="L13" s="15">
-        <f>[5]Main!$D$30</f>
+        <f>[6]Main!$D$30</f>
         <v>45559</v>
       </c>
       <c r="Q13" s="12">
-        <f>+[5]Main!$C$35</f>
+        <f>+[6]Main!$C$35</f>
         <v>3.1948131495535712</v>
       </c>
       <c r="R13" s="12">
-        <f>+[5]Main!$C$36</f>
+        <f>+[6]Main!$C$36</f>
         <v>2.6442251407476842</v>
       </c>
       <c r="S13" s="12">
-        <f>+[5]Main!$C$38</f>
+        <f>+[6]Main!$C$38</f>
         <v>15.436558542879432</v>
       </c>
       <c r="U13" s="14">
-        <f>+'[5]Financial Model'!$F$42</f>
+        <f>+'[6]Financial Model'!$F$42</f>
         <v>0.23750000000000002</v>
       </c>
       <c r="V13" s="14">
-        <f>+'[5]Financial Model'!$F$43</f>
+        <f>+'[6]Financial Model'!$F$43</f>
         <v>7.9166666666666677E-2</v>
       </c>
       <c r="W13" s="14">
-        <f>+'[5]Financial Model'!$F$44</f>
+        <f>+'[6]Financial Model'!$F$44</f>
         <v>5.2777777777777792E-2</v>
       </c>
       <c r="X13" s="14">
-        <f>+'[5]Financial Model'!$F$45</f>
+        <f>+'[6]Financial Model'!$F$45</f>
         <v>0.29629629629629622</v>
       </c>
       <c r="Z13" s="14">
-        <f>+'[5]Financial Model'!$F$30</f>
+        <f>+'[6]Financial Model'!$F$30</f>
         <v>0.61254199328107539</v>
       </c>
       <c r="AA13" s="14">
-        <f>+'[5]Financial Model'!$K$30</f>
+        <f>+'[6]Financial Model'!$K$30</f>
         <v>0.41487498602675421</v>
       </c>
       <c r="AB13" s="14">
-        <f>+'[5]Financial Model'!$J$30</f>
+        <f>+'[6]Financial Model'!$J$30</f>
         <v>0.33624730593867169</v>
       </c>
       <c r="AC13" s="2" t="s">
         <v>46</v>
       </c>
       <c r="AF13" s="2">
-        <f>+[5]Main!$C$27</f>
+        <f>+[6]Main!$C$27</f>
         <v>115</v>
       </c>
       <c r="AG13" s="2">
-        <f>+[5]Main!$C$24</f>
+        <f>+[6]Main!$C$24</f>
         <v>2012</v>
       </c>
       <c r="AH13" s="30">
-        <f>+[5]Main!$C$25</f>
+        <f>+[6]Main!$C$25</f>
         <v>45444</v>
       </c>
       <c r="AI13" s="2" t="str">
-        <f>[5]Main!$C$23</f>
+        <f>[6]Main!$C$23</f>
         <v>Cambridge, UK</v>
       </c>
       <c r="AK13" s="2" t="s">
@@ -2237,6 +2350,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="L3:L1048576">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>IF(LEFT(B3,1)="$",(TODAY()-L3)&gt;90,IF(LEFT(B3,1)="£",(TODAY()-L3)&gt;180,""))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{AFCC0C36-695A-4698-B366-E9445F7B4F63}"/>
     <hyperlink ref="B6" r:id="rId2" xr:uid="{1AA14988-C4F2-405C-BA9D-FBCA3DA35146}"/>
@@ -2259,7 +2377,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
$SPOT data backfill, more metrics
</commit_message>
<xml_diff>
--- a/Overview - Tech.xlsx
+++ b/Overview - Tech.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21496D18-E581-452E-968A-384D244EE95C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02348E5-F20D-4E27-A3D9-E305FDE51388}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1635" yWindow="1950" windowWidth="27165" windowHeight="14100" xr2:uid="{AFC643F4-9510-457F-8BC2-75D95EE8546E}"/>
   </bookViews>
@@ -30,15 +30,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -488,7 +479,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -627,7 +618,125 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Financial Model"/>
+      <sheetName val="Data Visualisation"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="C6">
+            <v>400.68</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>201</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8">
+            <v>80536.680000000008</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>5959</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>74577.680000000008</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="C23" t="str">
+            <v>Stockholm, Sweden</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="C24">
+            <v>2006</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="C25">
+            <v>2018</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="C27">
+            <v>626</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="C28">
+            <v>9123</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="C30" t="str">
+            <v>Q224</v>
+          </cell>
+          <cell r="D30">
+            <v>45480</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="C35">
+            <v>1.8383569335605636</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="C36">
+            <v>18.559875002592591</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="21">
+          <cell r="P21">
+            <v>0.19830028328611893</v>
+          </cell>
+          <cell r="Z21">
+            <v>0.21297062474141493</v>
+          </cell>
+          <cell r="AA21">
+            <v>0.12961541741280813</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="P24">
+            <v>0.29209351195166799</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="P25">
+            <v>6.9871289729445757E-2</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="P26">
+            <v>7.1972681901759913E-2</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="P27">
+            <v>-1.4814814814814815E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -754,8 +863,8 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -859,8 +968,8 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -970,8 +1079,220 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Financial Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="C6">
+            <v>9.8859999999999992</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>1016</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>-792</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="C24">
+            <v>1981</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="C25">
+            <v>1989</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="C26">
+            <v>11565</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="C27" t="str">
+            <v>H124</v>
+          </cell>
+          <cell r="D27">
+            <v>45428</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="C32">
+            <v>26.149764972535884</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="C33">
+            <v>4.4660631391729657</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="C34">
+            <v>9.2317794117647036</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="20">
+          <cell r="M20">
+            <v>0.92881944444444442</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="M21">
+            <v>0.18663194444444445</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="M22">
+            <v>0.13541666666666666</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="M23">
+            <v>0.23152709359605911</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="M25">
+            <v>5.9797608095676136E-2</v>
+          </cell>
+          <cell r="U25">
+            <v>-2.9952706253284278E-2</v>
+          </cell>
+          <cell r="V25">
+            <v>5.4712892741061836E-2</v>
+          </cell>
+          <cell r="W25">
+            <v>0.1217257318952234</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Financial Model"/>
+      <sheetName val="Data Visualisation"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="C6">
+            <v>3.33</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>193.41571500000001</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>26.295999999999999</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="C23" t="str">
+            <v>Cambridge, UK</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="C24">
+            <v>2012</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="C25">
+            <v>45444</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="C27">
+            <v>115</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="C30" t="str">
+            <v>H124</v>
+          </cell>
+          <cell r="D30">
+            <v>45559</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="C35">
+            <v>3.1948131495535712</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="C36">
+            <v>2.6442251407476842</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="C38">
+            <v>15.436558542879432</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="30">
+          <cell r="F30">
+            <v>0.61254199328107539</v>
+          </cell>
+          <cell r="J30">
+            <v>0.33624730593867169</v>
+          </cell>
+          <cell r="K30">
+            <v>0.41487498602675421</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="F42">
+            <v>0.23750000000000002</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="F43">
+            <v>7.9166666666666677E-2</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="F44">
+            <v>5.2777777777777792E-2</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="F45">
+            <v>0.29629629629629622</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -993,319 +1314,6 @@
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Financial Model"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="6">
-          <cell r="C6">
-            <v>9.8859999999999992</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7">
-            <v>1016</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>-792</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="C24">
-            <v>1981</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="C25">
-            <v>1989</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="C26">
-            <v>11565</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="C27" t="str">
-            <v>H124</v>
-          </cell>
-          <cell r="D27">
-            <v>45428</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="C32">
-            <v>26.149764972535884</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="C33">
-            <v>4.4660631391729657</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="C34">
-            <v>9.2317794117647036</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="20">
-          <cell r="M20">
-            <v>0.92881944444444442</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="M21">
-            <v>0.18663194444444445</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="M22">
-            <v>0.13541666666666666</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="M23">
-            <v>0.23152709359605911</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="M25">
-            <v>5.9797608095676136E-2</v>
-          </cell>
-          <cell r="U25">
-            <v>-2.9952706253284278E-2</v>
-          </cell>
-          <cell r="V25">
-            <v>5.4712892741061836E-2</v>
-          </cell>
-          <cell r="W25">
-            <v>0.1217257318952234</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Financial Model"/>
-      <sheetName val="Data Visualisation"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="6">
-          <cell r="C6">
-            <v>3.33</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7">
-            <v>193.41571500000001</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>26.295999999999999</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="C23" t="str">
-            <v>Cambridge, UK</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="C24">
-            <v>2012</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="C25">
-            <v>45444</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="C27">
-            <v>115</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="C30" t="str">
-            <v>H124</v>
-          </cell>
-          <cell r="D30">
-            <v>45559</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="C35">
-            <v>3.1948131495535712</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="C36">
-            <v>2.6442251407476842</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="C38">
-            <v>15.436558542879432</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="30">
-          <cell r="F30">
-            <v>0.61254199328107539</v>
-          </cell>
-          <cell r="J30">
-            <v>0.33624730593867169</v>
-          </cell>
-          <cell r="K30">
-            <v>0.41487498602675421</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="F42">
-            <v>0.23750000000000002</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="F43">
-            <v>7.9166666666666677E-2</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="F44">
-            <v>5.2777777777777792E-2</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="F45">
-            <v>0.29629629629629622</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Financial Model"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="6">
-          <cell r="C6">
-            <v>400.68</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7">
-            <v>201</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="C8">
-            <v>80536.680000000008</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>5959</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12">
-            <v>74577.680000000008</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="C23" t="str">
-            <v>Stockholm, Sweden</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="C24">
-            <v>2006</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="C30" t="str">
-            <v>Q224</v>
-          </cell>
-          <cell r="D30">
-            <v>45480</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="C35">
-            <v>1.8383569335605636</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="C36">
-            <v>18.559875002592591</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="19">
-          <cell r="P19">
-            <v>0.19830028328611893</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="P22">
-            <v>0.29209351195166799</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="P23">
-            <v>6.9871289729445757E-2</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="P24">
-            <v>7.1972681901759913E-2</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="P25">
-            <v>-1.4814814814814815E-2</v>
-          </cell>
-        </row>
-      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1614,7 +1622,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R5" sqref="R5"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1888,67 +1896,87 @@
         <v>33</v>
       </c>
       <c r="F4" s="10">
-        <f>[8]Main!$C$6</f>
+        <f>[2]Main!$C$6</f>
         <v>400.68</v>
       </c>
       <c r="G4" s="8">
-        <f>[8]Main!$C$7</f>
+        <f>[2]Main!$C$7</f>
         <v>201</v>
       </c>
       <c r="H4" s="8">
-        <f>[8]Main!$C$8</f>
+        <f>[2]Main!$C$8</f>
         <v>80536.680000000008</v>
       </c>
       <c r="I4" s="8">
-        <f>[8]Main!$C$11*Currencies!D3</f>
+        <f>[2]Main!$C$11*Currencies!D3</f>
         <v>4583.8461538461534</v>
       </c>
       <c r="J4" s="8">
-        <f>[8]Main!$C$12</f>
+        <f>[2]Main!$C$12</f>
         <v>74577.680000000008</v>
       </c>
       <c r="K4" s="2" t="str">
-        <f>[8]Main!$C$30</f>
+        <f>[2]Main!$C$30</f>
         <v>Q224</v>
       </c>
       <c r="L4" s="15">
-        <f>[8]Main!$D$30</f>
+        <f>[2]Main!$D$30</f>
         <v>45480</v>
       </c>
       <c r="Q4" s="12">
-        <f>[8]Main!$C$35</f>
+        <f>[2]Main!$C$35</f>
         <v>1.8383569335605636</v>
       </c>
       <c r="R4" s="12">
-        <f>[8]Main!$C$36</f>
+        <f>[2]Main!$C$36</f>
         <v>18.559875002592591</v>
       </c>
       <c r="U4" s="14">
-        <f>'[8]Financial Model'!$P$22</f>
+        <f>'[2]Financial Model'!$P$24</f>
         <v>0.29209351195166799</v>
       </c>
       <c r="V4" s="14">
-        <f>'[8]Financial Model'!$P$23</f>
+        <f>'[2]Financial Model'!$P$25</f>
         <v>6.9871289729445757E-2</v>
       </c>
       <c r="W4" s="14">
-        <f>'[8]Financial Model'!$P$24</f>
+        <f>'[2]Financial Model'!$P$26</f>
         <v>7.1972681901759913E-2</v>
       </c>
       <c r="X4" s="14">
-        <f>'[8]Financial Model'!$P$25</f>
+        <f>'[2]Financial Model'!$P$27</f>
         <v>-1.4814814814814815E-2</v>
       </c>
       <c r="Z4" s="14">
-        <f>'[8]Financial Model'!$P$19</f>
+        <f>'[2]Financial Model'!$P$21</f>
         <v>0.19830028328611893</v>
       </c>
+      <c r="AA4" s="14">
+        <f>'[2]Financial Model'!$AA$21</f>
+        <v>0.12961541741280813</v>
+      </c>
+      <c r="AB4" s="14">
+        <f>'[2]Financial Model'!$Z$21</f>
+        <v>0.21297062474141493</v>
+      </c>
+      <c r="AE4" s="20">
+        <f>+[2]Main!$C$27/30</f>
+        <v>20.866666666666667</v>
+      </c>
+      <c r="AF4" s="20">
+        <f>+[2]Main!$C$28</f>
+        <v>9123</v>
+      </c>
       <c r="AG4" s="2">
-        <f>[8]Main!$C$24</f>
+        <f>[2]Main!$C$24</f>
         <v>2006</v>
       </c>
+      <c r="AH4" s="2">
+        <f>+[2]Main!$C$25</f>
+        <v>2018</v>
+      </c>
       <c r="AI4" s="2" t="str">
-        <f>[8]Main!$C$23</f>
+        <f>[2]Main!$C$23</f>
         <v>Stockholm, Sweden</v>
       </c>
       <c r="AK4" s="2" t="s">
@@ -1972,104 +2000,104 @@
         <v>33</v>
       </c>
       <c r="F5" s="10">
-        <f>+[2]Main!$C$6</f>
+        <f>+[3]Main!$C$6</f>
         <v>51.68</v>
       </c>
       <c r="G5" s="8">
-        <f>+[2]Main!$C$7</f>
+        <f>+[3]Main!$C$7</f>
         <v>641.81399999999996</v>
       </c>
       <c r="H5" s="8">
-        <f>+[2]Main!$C$8</f>
+        <f>+[3]Main!$C$8</f>
         <v>33168.947520000002</v>
       </c>
       <c r="I5" s="8">
-        <f>+[2]Main!$C$11</f>
+        <f>+[3]Main!$C$11</f>
         <v>2595.5510000000004</v>
       </c>
       <c r="J5" s="8">
-        <f>+[2]Main!$C$12</f>
+        <f>+[3]Main!$C$12</f>
         <v>30573.396520000002</v>
       </c>
       <c r="K5" s="2" t="str">
-        <f>+[2]Main!$G$11</f>
+        <f>+[3]Main!$G$11</f>
         <v>Q324</v>
       </c>
       <c r="L5" s="15">
-        <f>+[2]Main!$H$11</f>
+        <f>+[3]Main!$H$11</f>
         <v>45596</v>
       </c>
       <c r="M5" s="22">
-        <f>+'[2]Financial Model'!$AX$26</f>
+        <f>+'[3]Financial Model'!$AX$26</f>
         <v>71.486963060421459</v>
       </c>
       <c r="N5" s="18">
-        <f>+'[2]Financial Model'!$AX$28</f>
+        <f>+'[3]Financial Model'!$AX$28</f>
         <v>0.38326166912580217</v>
       </c>
       <c r="O5" s="18">
-        <f>+'[2]Financial Model'!$AX$22</f>
+        <f>+'[3]Financial Model'!$AX$22</f>
         <v>0.09</v>
       </c>
       <c r="Q5" s="12">
-        <f>+[2]Main!$G$16</f>
+        <f>+[3]Main!$G$16</f>
         <v>523.51896884519317</v>
       </c>
       <c r="R5" s="12">
-        <f>+[2]Main!$G$17</f>
+        <f>+[3]Main!$G$17</f>
         <v>11.261920977309074</v>
       </c>
       <c r="S5" s="12">
-        <f>+[2]Main!$G$18</f>
+        <f>+[3]Main!$G$18</f>
         <v>-27.750520841528012</v>
       </c>
       <c r="U5" s="14">
-        <f>+'[2]Financial Model'!$T$22</f>
+        <f>+'[3]Financial Model'!$T$22</f>
         <v>0.77778685524927171</v>
       </c>
       <c r="V5" s="14">
-        <f>+'[2]Financial Model'!$T$23</f>
+        <f>+'[3]Financial Model'!$T$23</f>
         <v>-0.26629832028229189</v>
       </c>
       <c r="W5" s="14">
-        <f>+'[2]Financial Model'!$T$24</f>
+        <f>+'[3]Financial Model'!$T$24</f>
         <v>-0.23188027884500237</v>
       </c>
       <c r="X5" s="14">
-        <f>+'[2]Financial Model'!$T$25</f>
+        <f>+'[3]Financial Model'!$T$25</f>
         <v>-5.311828476229569E-4</v>
       </c>
       <c r="Z5" s="14">
-        <f>+'[2]Financial Model'!$T$28</f>
+        <f>+'[3]Financial Model'!$T$28</f>
         <v>0.31255526862387373</v>
       </c>
       <c r="AA5" s="14"/>
       <c r="AB5" s="14">
-        <f>+'[2]Financial Model'!$AF$28</f>
+        <f>+'[3]Financial Model'!$AF$28</f>
         <v>0.15937579623808262</v>
       </c>
       <c r="AC5" s="14">
-        <f>+'[2]Financial Model'!$AE$28</f>
+        <f>+'[3]Financial Model'!$AE$28</f>
         <v>1.0772942519902369</v>
       </c>
       <c r="AE5" s="20">
-        <f>+[2]Main!$G$9</f>
+        <f>+[3]Main!$G$9</f>
         <v>79.5</v>
       </c>
       <c r="AF5" s="20">
-        <f>+[2]Main!$G$10</f>
+        <f>+[3]Main!$G$10</f>
         <v>2457</v>
       </c>
       <c r="AG5" s="2">
-        <f>+[2]Main!$G$8</f>
+        <f>+[3]Main!$G$8</f>
         <v>2004</v>
       </c>
       <c r="AH5" s="2">
-        <f>+[2]Main!$G$7</f>
+        <f>+[3]Main!$G$7</f>
         <v>2021</v>
       </c>
       <c r="AI5" s="2" t="str">
-        <f>+[2]Main!$G$6</f>
+        <f>+[3]Main!$G$6</f>
         <v>San Mateo, CA</v>
       </c>
       <c r="AK5" s="2" t="s">
@@ -2093,55 +2121,55 @@
         <v>33</v>
       </c>
       <c r="F6" s="10">
-        <f>+[3]Main!$C$6</f>
+        <f>+[4]Main!$C$6</f>
         <v>129.71</v>
       </c>
       <c r="G6" s="8">
-        <f>+[3]Main!$C$7</f>
+        <f>+[4]Main!$C$7</f>
         <v>169.16992200000001</v>
       </c>
       <c r="H6" s="8">
-        <f>+[3]Main!$C$8</f>
+        <f>+[4]Main!$C$8</f>
         <v>21943.030582620002</v>
       </c>
       <c r="I6" s="8">
-        <f>+[3]Main!$C$11</f>
+        <f>+[4]Main!$C$11</f>
         <v>1744.9669999999999</v>
       </c>
       <c r="J6" s="8">
-        <f>+[3]Main!$C$12</f>
+        <f>+[4]Main!$C$12</f>
         <v>20198.063582620001</v>
       </c>
       <c r="K6" s="2" t="str">
-        <f>+[3]Main!$C$32</f>
+        <f>+[4]Main!$C$32</f>
         <v>Q324</v>
       </c>
       <c r="L6" s="15">
-        <f>+[3]Main!$D$32</f>
+        <f>+[4]Main!$D$32</f>
         <v>45594</v>
       </c>
       <c r="Q6" s="12">
-        <f>+[3]Main!$C$37</f>
+        <f>+[4]Main!$C$37</f>
         <v>11.095743232541535</v>
       </c>
       <c r="U6" s="14">
-        <f>+'[3]Financial Model'!$I$18</f>
+        <f>+'[4]Financial Model'!$I$18</f>
         <v>0.90049404192897387</v>
       </c>
       <c r="V6" s="14">
-        <f>+'[3]Financial Model'!$I$19</f>
+        <f>+'[4]Financial Model'!$I$19</f>
         <v>1.9589437090750374E-2</v>
       </c>
       <c r="W6" s="14">
-        <f>+'[3]Financial Model'!$I$20</f>
+        <f>+'[4]Financial Model'!$I$20</f>
         <v>8.5611925902322611E-2</v>
       </c>
       <c r="X6" s="14">
-        <f>+'[3]Financial Model'!$I$21</f>
+        <f>+'[4]Financial Model'!$I$21</f>
         <v>-1.0405477980665956E-3</v>
       </c>
       <c r="Z6" s="14">
-        <f>+'[3]Financial Model'!$I$24</f>
+        <f>+'[4]Financial Model'!$I$24</f>
         <v>0.67873527767604136</v>
       </c>
       <c r="AB6" s="2" t="s">
@@ -2151,23 +2179,23 @@
         <v>46</v>
       </c>
       <c r="AE6" s="20">
-        <f>+[3]Main!$C$29</f>
+        <f>+[4]Main!$C$29</f>
         <v>97.2</v>
       </c>
       <c r="AF6" s="20">
-        <f>+[3]Main!$C$30</f>
+        <f>+[4]Main!$C$30</f>
         <v>2013</v>
       </c>
       <c r="AG6" s="2">
-        <f>+[3]Main!$C$25</f>
+        <f>+[4]Main!$C$25</f>
         <v>2005</v>
       </c>
       <c r="AH6" s="2">
-        <f>+[3]Main!$C$26</f>
+        <f>+[4]Main!$C$26</f>
         <v>2024</v>
       </c>
       <c r="AI6" s="2" t="str">
-        <f>+[3]Main!$C$24</f>
+        <f>+[4]Main!$C$24</f>
         <v>San Fransisco, CA</v>
       </c>
       <c r="AK6" s="2" t="s">
@@ -2191,83 +2219,83 @@
         <v>33</v>
       </c>
       <c r="F7" s="10">
-        <f>+[4]Main!$C$6</f>
+        <f>+[5]Main!$C$6</f>
         <v>36.5</v>
       </c>
       <c r="G7" s="8">
-        <f>+[4]Main!$C$7</f>
+        <f>+[5]Main!$C$7</f>
         <v>563</v>
       </c>
       <c r="H7" s="8">
-        <f>+[4]Main!$C$8</f>
+        <f>+[5]Main!$C$8</f>
         <v>20549.5</v>
       </c>
       <c r="I7" s="8">
-        <f>+[4]Main!$C$11</f>
+        <f>+[5]Main!$C$11</f>
         <v>1272</v>
       </c>
       <c r="J7" s="8">
-        <f>+[4]Main!$C$12</f>
+        <f>+[5]Main!$C$12</f>
         <v>19277.5</v>
       </c>
       <c r="K7" s="2" t="str">
-        <f>+[4]Main!$C$30</f>
+        <f>+[5]Main!$C$30</f>
         <v>Q324</v>
       </c>
       <c r="L7" s="15">
-        <f>+[4]Main!$D$30</f>
+        <f>+[5]Main!$D$30</f>
         <v>45603</v>
       </c>
       <c r="Q7" s="12">
-        <f>+[4]Main!$C$35</f>
+        <f>+[5]Main!$C$35</f>
         <v>14.471478873239437</v>
       </c>
       <c r="R7" s="12">
-        <f>+[4]Main!$C$36</f>
+        <f>+[5]Main!$C$36</f>
         <v>4.4116573636753973</v>
       </c>
       <c r="U7" s="14">
-        <f>+'[4]Financial Model'!$M$28</f>
+        <f>+'[5]Financial Model'!$M$28</f>
         <v>0.24674329501915709</v>
       </c>
       <c r="V7" s="14">
-        <f>+'[4]Financial Model'!$M$29</f>
+        <f>+'[5]Financial Model'!$M$29</f>
         <v>2.6053639846743294E-2</v>
       </c>
       <c r="W7" s="14">
-        <f>+'[4]Financial Model'!$M$30</f>
+        <f>+'[5]Financial Model'!$M$30</f>
         <v>4.2911877394636012E-2</v>
       </c>
       <c r="X7" s="14">
-        <f>+'[4]Financial Model'!$M$31</f>
+        <f>+'[5]Financial Model'!$M$31</f>
         <v>1.7543859649122806E-2</v>
       </c>
       <c r="Z7" s="14">
-        <f>+'[4]Financial Model'!$M$33</f>
+        <f>+'[5]Financial Model'!$M$33</f>
         <v>0.26453488372093026</v>
       </c>
       <c r="AA7" s="14">
-        <f>+'[4]Financial Model'!$U$33</f>
+        <f>+'[5]Financial Model'!$U$33</f>
         <v>0.41523251556206509</v>
       </c>
       <c r="AB7" s="14">
-        <f>+'[4]Financial Model'!$T$33</f>
+        <f>+'[5]Financial Model'!$T$33</f>
         <v>0.6017595307917889</v>
       </c>
       <c r="AF7" s="20">
-        <f>+[4]Main!$C$28</f>
+        <f>+[5]Main!$C$28</f>
         <v>5500</v>
       </c>
       <c r="AG7" s="2">
-        <f>+[4]Main!$C$24</f>
+        <f>+[5]Main!$C$24</f>
         <v>2011</v>
       </c>
       <c r="AH7" s="2">
-        <f>+[4]Main!$C$25</f>
+        <f>+[5]Main!$C$25</f>
         <v>2021</v>
       </c>
       <c r="AI7" s="2" t="str">
-        <f>+[4]Main!$C$23</f>
+        <f>+[5]Main!$C$23</f>
         <v>Boston, MA</v>
       </c>
       <c r="AL7" s="2" t="s">
@@ -2501,11 +2529,11 @@
         <v>70</v>
       </c>
       <c r="K12" s="2" t="str">
-        <f>+[5]Main!$C$28</f>
+        <f>+[8]Main!$C$28</f>
         <v>Q123</v>
       </c>
       <c r="L12" s="15">
-        <f>+[5]Main!$D$28</f>
+        <f>+[8]Main!$D$28</f>
         <v>45055</v>
       </c>
     </row>
@@ -2557,7 +2585,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Further work looking at £BOKU
</commit_message>
<xml_diff>
--- a/Overview - Tech.xlsx
+++ b/Overview - Tech.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375DF7E1-2976-4406-99C4-F6F3879F8643}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EC27C8-226D-4F00-9C61-9A7CDCDDB98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AFC643F4-9510-457F-8BC2-75D95EE8546E}"/>
   </bookViews>
@@ -39,6 +39,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -6996,7 +7005,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -7140,7 +7149,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink10.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -7268,7 +7277,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink11.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -7368,7 +7377,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -7502,7 +7511,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink13.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -7615,75 +7624,11 @@
 </file>
 
 <file path=xl/externalLinks/externalLink14.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="6">
-          <cell r="C6">
-            <v>7.0000000000000001E-3</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="C7">
-            <v>275</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="C11">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="C23" t="str">
-            <v>Weybridge, UK</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="C34">
-            <v>4</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink15.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Financial Model"/>
-      <sheetName val="Historical Projections"/>
-      <sheetName val="Price History"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="28">
-          <cell r="C28" t="str">
-            <v>Q123</v>
-          </cell>
-          <cell r="D28">
-            <v>45055</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink16.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Financial Model"/>
@@ -7792,8 +7737,75 @@
 </externalLink>
 </file>
 
+<file path=xl/externalLinks/externalLink15.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="C6">
+            <v>7.0000000000000001E-3</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>275</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="C23" t="str">
+            <v>Weybridge, UK</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="C34">
+            <v>4</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink16.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Financial Model"/>
+      <sheetName val="Historical Projections"/>
+      <sheetName val="Price History"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="28">
+          <cell r="C28" t="str">
+            <v>Q123</v>
+          </cell>
+          <cell r="D28">
+            <v>45055</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -7914,14 +7926,14 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -8057,7 +8069,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -8185,7 +8197,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -8309,7 +8321,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -8445,7 +8457,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -8550,7 +8562,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -8661,7 +8673,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -9069,7 +9081,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I18" sqref="I18"/>
+      <selection pane="bottomRight" activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -10704,11 +10716,11 @@
         <v>33</v>
       </c>
       <c r="F16" s="10">
-        <f>+[16]Main!$C$6*Currencies!$C$3</f>
+        <f>+[14]Main!$C$6*Currencies!$C$3</f>
         <v>2.0939100000000002</v>
       </c>
       <c r="G16" s="8">
-        <f>+[16]Main!$C$7</f>
+        <f>+[14]Main!$C$7</f>
         <v>303.02861300000001</v>
       </c>
       <c r="H16" s="8">
@@ -10716,7 +10728,7 @@
         <v>634.51464304683009</v>
       </c>
       <c r="I16" s="8">
-        <f>+[16]Main!$C$11*Currencies!C3</f>
+        <f>+[14]Main!$C$11*Currencies!C3</f>
         <v>143.40719900000002</v>
       </c>
       <c r="J16" s="8">
@@ -10724,63 +10736,63 @@
         <v>491.1074440468301</v>
       </c>
       <c r="K16" s="2" t="str">
-        <f>+[16]Main!$C$30</f>
+        <f>+[14]Main!$C$30</f>
         <v>H124</v>
       </c>
       <c r="L16" s="13">
-        <f>+[16]Main!$D$30</f>
+        <f>+[14]Main!$D$30</f>
         <v>45536</v>
       </c>
       <c r="Q16" s="30">
-        <f>+[16]Main!$C$35</f>
+        <f>+[14]Main!$C$35</f>
         <v>4.4631448966950336</v>
       </c>
       <c r="R16" s="30">
-        <f>+[16]Main!$C$36</f>
+        <f>+[14]Main!$C$36</f>
         <v>6.7280098883751904</v>
       </c>
       <c r="S16" s="30">
-        <f>+[16]Main!$C$38</f>
+        <f>+[14]Main!$C$38</f>
         <v>84.972354260847055</v>
       </c>
       <c r="T16" s="30">
-        <f>+[16]Main!$C$40</f>
+        <f>+[14]Main!$C$40</f>
         <v>15.357141210745286</v>
       </c>
       <c r="V16" s="12">
-        <f>+'[16]Financial Model'!$Q$22</f>
+        <f>+'[14]Financial Model'!$Q$22</f>
         <v>0.9711318839353692</v>
       </c>
       <c r="W16" s="12">
-        <f>+'[16]Financial Model'!$Q$23</f>
+        <f>+'[14]Financial Model'!$Q$23</f>
         <v>-8.3749259791895941E-3</v>
       </c>
       <c r="X16" s="12">
-        <f>+'[16]Financial Model'!$Q$24</f>
+        <f>+'[14]Financial Model'!$Q$24</f>
         <v>-2.2608070383216328E-2</v>
       </c>
       <c r="AA16" s="12">
-        <f>+'[16]Financial Model'!$Q$19</f>
+        <f>+'[14]Financial Model'!$Q$19</f>
         <v>0.2386441033163933</v>
       </c>
       <c r="AB16" s="12">
-        <f>+'[16]Financial Model'!$AC$19</f>
+        <f>+'[14]Financial Model'!$AC$19</f>
         <v>0.29728373376827033</v>
       </c>
       <c r="AH16" s="2">
-        <f>+[16]Main!$C$24</f>
+        <f>+[14]Main!$C$24</f>
         <v>2008</v>
       </c>
       <c r="AI16" s="2">
-        <f>+[16]Main!$C$25</f>
+        <f>+[14]Main!$C$25</f>
         <v>2017</v>
       </c>
       <c r="AJ16" s="2" t="str">
-        <f>+[16]Main!$C$23</f>
+        <f>+[14]Main!$C$23</f>
         <v>San Francisco, CA</v>
       </c>
       <c r="AL16" s="2">
-        <f>+[16]Main!$C$41</f>
+        <f>+[14]Main!$C$41</f>
         <v>38</v>
       </c>
       <c r="AN16" s="2" t="s">
@@ -10790,11 +10802,11 @@
         <v>2238</v>
       </c>
       <c r="AQ16" s="2" t="str">
-        <f>+[16]Main!$C$16</f>
+        <f>+[14]Main!$C$16</f>
         <v>Stuart Neal</v>
       </c>
       <c r="AR16" s="2">
-        <f ca="1">DATEDIF( [16]Main!$A$16, TODAY(), "y")</f>
+        <f ca="1">DATEDIF( [14]Main!$A$16, TODAY(), "y")</f>
         <v>0</v>
       </c>
       <c r="AS16" s="2" t="s">
@@ -10815,11 +10827,11 @@
         <v>51</v>
       </c>
       <c r="F17" s="10">
-        <f>+[14]Sheet1!$C$6*Currencies!C3</f>
+        <f>+[15]Sheet1!$C$6*Currencies!C3</f>
         <v>9.1000000000000004E-3</v>
       </c>
       <c r="G17" s="8">
-        <f>+[14]Sheet1!$C$7</f>
+        <f>+[15]Sheet1!$C$7</f>
         <v>275</v>
       </c>
       <c r="H17" s="8">
@@ -10827,7 +10839,7 @@
         <v>2.5024999999999999</v>
       </c>
       <c r="I17" s="8">
-        <f>+[14]Sheet1!$C$11*Currencies!C3</f>
+        <f>+[15]Sheet1!$C$11*Currencies!C3</f>
         <v>0</v>
       </c>
       <c r="J17" s="8">
@@ -10835,11 +10847,11 @@
         <v>2.5024999999999999</v>
       </c>
       <c r="AJ17" s="2" t="str">
-        <f>+[14]Sheet1!$C$23</f>
+        <f>+[15]Sheet1!$C$23</f>
         <v>Weybridge, UK</v>
       </c>
       <c r="AL17" s="2">
-        <f>+[14]Sheet1!$C$34</f>
+        <f>+[15]Sheet1!$C$34</f>
         <v>4</v>
       </c>
       <c r="AN17" s="2" t="s">
@@ -10859,11 +10871,11 @@
         <v>68</v>
       </c>
       <c r="K20" s="2" t="str">
-        <f>+[15]Main!$C$28</f>
+        <f>+[16]Main!$C$28</f>
         <v>Q123</v>
       </c>
       <c r="L20" s="13">
-        <f>+[15]Main!$D$28</f>
+        <f>+[16]Main!$D$28</f>
         <v>45055</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Further look into £BOKU, VERY BASIC DCF
</commit_message>
<xml_diff>
--- a/Overview - Tech.xlsx
+++ b/Overview - Tech.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EC27C8-226D-4F00-9C61-9A7CDCDDB98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8B1523-8310-44E9-917E-415B0EFC6FB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AFC643F4-9510-457F-8BC2-75D95EE8546E}"/>
   </bookViews>
@@ -39,15 +39,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -7005,7 +6996,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -7149,7 +7140,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink10.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -7277,7 +7268,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink11.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -7377,7 +7368,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -7511,7 +7502,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink13.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -7624,11 +7615,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink14.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Financial Model"/>
@@ -7712,6 +7700,12 @@
           <cell r="Q19">
             <v>0.2386441033163933</v>
           </cell>
+          <cell r="AA19">
+            <v>0.22628630190418786</v>
+          </cell>
+          <cell r="AB19">
+            <v>-7.8088628641654112E-2</v>
+          </cell>
           <cell r="AC19">
             <v>0.29728373376827033</v>
           </cell>
@@ -7738,7 +7732,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink15.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -7777,7 +7771,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink16.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -7805,7 +7799,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -7933,7 +7927,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -8069,7 +8063,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -8197,7 +8191,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -8321,7 +8315,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -8457,7 +8451,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -8562,7 +8556,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -8673,7 +8667,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Main"/>
@@ -9081,7 +9075,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="U17" sqref="U17"/>
+      <selection pane="bottomRight" activeCell="AE16" sqref="AE16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -10778,6 +10772,14 @@
       <c r="AB16" s="12">
         <f>+'[14]Financial Model'!$AC$19</f>
         <v>0.29728373376827033</v>
+      </c>
+      <c r="AC16" s="12">
+        <f>+'[14]Financial Model'!$AB$19</f>
+        <v>-7.8088628641654112E-2</v>
+      </c>
+      <c r="AD16" s="12">
+        <f>+'[14]Financial Model'!$AA$19</f>
+        <v>0.22628630190418786</v>
       </c>
       <c r="AH16" s="2">
         <f>+[14]Main!$C$24</f>

</xml_diff>